<commit_message>
Add new request based on geo dimensions
Pretty much all the same but intresting
</commit_message>
<xml_diff>
--- a/df-model/preliminary workload.xlsx
+++ b/df-model/preliminary workload.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
   <si>
     <t>RequestId</t>
   </si>
@@ -166,6 +166,54 @@
   </si>
   <si>
     <t>sick</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>What is the percentage of sick trees that are near a river ?</t>
+  </si>
+  <si>
+    <t>What is the percentage of sick trees that are near a building ?</t>
+  </si>
+  <si>
+    <t>How many trees are near a building ?</t>
+  </si>
+  <si>
+    <t>How many trees are near a river ?</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>Q18</t>
+  </si>
+  <si>
+    <t>What is the percentage of sick trees that are near a heliport ?</t>
+  </si>
+  <si>
+    <t>How many trees are near a heliport ?</t>
+  </si>
+  <si>
+    <t>What is the percentage of sick trees that are near a motorway ?</t>
+  </si>
+  <si>
+    <t>How many trees are near a motorway ?</t>
   </si>
 </sst>
 </file>
@@ -232,11 +280,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,20 +566,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -564,13 +613,37 @@
       <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -588,8 +661,32 @@
         <v>43</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -605,8 +702,16 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -620,8 +725,16 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -641,8 +754,16 @@
         <v>43</v>
       </c>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -662,8 +783,16 @@
         <v>43</v>
       </c>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -683,8 +812,16 @@
         <v>43</v>
       </c>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -704,8 +841,16 @@
         <v>43</v>
       </c>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -719,8 +864,16 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -734,8 +887,16 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -751,8 +912,16 @@
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -768,8 +937,16 @@
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -785,8 +962,16 @@
       <c r="K14" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -800,8 +985,16 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -821,8 +1014,16 @@
       <c r="K16" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -854,13 +1055,29 @@
       <c r="K17" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -874,8 +1091,24 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -909,8 +1142,24 @@
       <c r="K20" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -926,8 +1175,16 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -943,8 +1200,16 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -960,8 +1225,16 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -977,6 +1250,14 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -986,9 +1267,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1084,6 +1367,70 @@
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update mapping and preliminary workload
</commit_message>
<xml_diff>
--- a/df-model/preliminary workload.xlsx
+++ b/df-model/preliminary workload.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\Projet-Decisionnel-JVCTL\df-model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="formalization of requirements" sheetId="1" r:id="rId1"/>
     <sheet name="preliminary workload" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="98">
   <si>
     <t>RequestId</t>
   </si>
@@ -200,13 +205,127 @@
   </si>
   <si>
     <t>diseases</t>
+  </si>
+  <si>
+    <t>Q19</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>pollutionDate</t>
+  </si>
+  <si>
+    <t>pollutionStation</t>
+  </si>
+  <si>
+    <t>PollutionReading</t>
+  </si>
+  <si>
+    <t>PM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nitrogen dioxide </t>
+  </si>
+  <si>
+    <t>nitric oxide</t>
+  </si>
+  <si>
+    <t>ozone</t>
+  </si>
+  <si>
+    <t>benzene</t>
+  </si>
+  <si>
+    <t>benz(a)anthracene</t>
+  </si>
+  <si>
+    <t>benz(a)pyrene</t>
+  </si>
+  <si>
+    <t>benz(b)fluoranthene</t>
+  </si>
+  <si>
+    <t>benz(j)fluoranthene</t>
+  </si>
+  <si>
+    <t>benz(k)fluoranthene</t>
+  </si>
+  <si>
+    <t>dibenzo(a,h)anthracene</t>
+  </si>
+  <si>
+    <t>indeno(1,2,3-cd)pyrene</t>
+  </si>
+  <si>
+    <t>PM2,5</t>
+  </si>
+  <si>
+    <t>toluene</t>
+  </si>
+  <si>
+    <t>antimony</t>
+  </si>
+  <si>
+    <t>arsenic</t>
+  </si>
+  <si>
+    <t>barium</t>
+  </si>
+  <si>
+    <t>cadium</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>cobalt</t>
+  </si>
+  <si>
+    <t>copper</t>
+  </si>
+  <si>
+    <t>sulfur dioxide</t>
+  </si>
+  <si>
+    <t>ethylBenzene</t>
+  </si>
+  <si>
+    <t>m+p-xylene</t>
+  </si>
+  <si>
+    <t>manganese</t>
+  </si>
+  <si>
+    <t>mercury</t>
+  </si>
+  <si>
+    <t>nickel</t>
+  </si>
+  <si>
+    <t>o-xylene</t>
+  </si>
+  <si>
+    <t>lead</t>
+  </si>
+  <si>
+    <t>thallium</t>
+  </si>
+  <si>
+    <t>vanadium</t>
+  </si>
+  <si>
+    <t>zinc</t>
+  </si>
+  <si>
+    <t>What is the average quantity of a given pollutant by sector sector ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,8 +349,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +396,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -292,11 +432,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -306,8 +483,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,167 +776,189 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="9" t="s">
+      <c r="V1" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -750,99 +968,108 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" s="6" customFormat="1">
-      <c r="A6" s="4" t="s">
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="6" customFormat="1">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -851,13 +1078,16 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
-    </row>
-    <row r="8" spans="1:19" s="6" customFormat="1">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -867,20 +1097,25 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-    </row>
-    <row r="9" spans="1:19" s="6" customFormat="1">
-      <c r="A9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -899,23 +1134,26 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
-    </row>
-    <row r="10" spans="1:19" s="6" customFormat="1">
-      <c r="A10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="K10" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -924,21 +1162,22 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-    </row>
-    <row r="11" spans="1:19" s="6" customFormat="1">
-      <c r="A11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -949,13 +1188,16 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
-    </row>
-    <row r="12" spans="1:19" s="6" customFormat="1">
-      <c r="A12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -972,22 +1214,31 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
-    </row>
-    <row r="13" spans="1:19" s="6" customFormat="1">
-      <c r="A13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -995,13 +1246,18 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
-    </row>
-    <row r="14" spans="1:19" s="6" customFormat="1">
-      <c r="A14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1018,36 +1274,46 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="9" t="s">
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1057,9 +1323,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
         <v>32</v>
@@ -1072,17 +1336,18 @@
       <c r="S16" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="1" t="s">
+      <c r="T16" s="1"/>
+      <c r="U16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1110,7 +1375,9 @@
       <c r="L17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="N17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1123,17 +1390,20 @@
         <v>32</v>
       </c>
       <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="1" t="s">
+      <c r="T17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1148,17 +1418,18 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="1" t="s">
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1173,17 +1444,18 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="1" t="s">
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1198,17 +1470,18 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="1" t="s">
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1223,28 +1496,937 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:B15"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B53"/>
+    <mergeCell ref="A22:A53"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +2442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +2450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1276,7 +2458,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +2466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +2474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1300,7 +2482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1308,7 +2490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +2498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +2506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1332,7 +2514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1340,7 +2522,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1348,7 +2530,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1356,7 +2538,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1364,7 +2546,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -1372,7 +2554,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1380,7 +2562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
@@ -1388,12 +2570,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>